<commit_message>
Initial Commit - SocialMedia SafeSearch
</commit_message>
<xml_diff>
--- a/SocialMediaSafeSearch/Output/ImageDetails.xlsx
+++ b/SocialMediaSafeSearch/Output/ImageDetails.xlsx
@@ -1,20 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SimplyData\RPA\SocialMediaSafeSearch\Output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5992A31-2C35-49F6-A612-07ED1F1BF08B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{12625767-157A-49B6-AE1F-BD54B78C9003}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+  <si>
+    <t>D:\SimplyData\RPA\SocialMediaSafeSearch\Input\Adult.jpg</t>
+  </si>
+  <si>
+    <t>D:\SimplyData\RPA\SocialMediaSafeSearch\Input\Mountain.png</t>
+  </si>
+  <si>
+    <t>D:\SimplyData\RPA\SocialMediaSafeSearch\Input\Murder.jpg</t>
+  </si>
+  <si>
+    <t>ImagePath</t>
+  </si>
   <si>
     <t>Adult</t>
   </si>
@@ -28,13 +51,22 @@
     <t>Medical</t>
   </si>
   <si>
-    <t>ImagePath</t>
+    <t>VERY_UNLIKELY</t>
+  </si>
+  <si>
+    <t>POSSIBLE</t>
+  </si>
+  <si>
+    <t>VERY_LIKELY</t>
+  </si>
+  <si>
+    <t>UNLIKELY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -71,7 +103,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -94,44 +126,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -159,14 +191,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -194,6 +243,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -205,198 +271,226 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64180483-0E46-48B2-AFF2-73D2632BFF68}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="73.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.28515625" customWidth="1"/>
+    <col min="2" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>